<commit_message>
Ermannos R Artefakte übernommen
</commit_message>
<xml_diff>
--- a/data/output/BDA6_SCHULE_Gemeinden_LU_Ranked.xlsx
+++ b/data/output/BDA6_SCHULE_Gemeinden_LU_Ranked.xlsx
@@ -184,37 +184,47 @@
       </c>
       <c r="Y1" t="inlineStr">
         <is>
+          <t>AuslaenderAnteil</t>
+        </is>
+      </c>
+      <c r="Z1" t="inlineStr">
+        <is>
           <t>GesamtRank</t>
         </is>
       </c>
-      <c r="Z1" t="inlineStr">
+      <c r="AA1" t="inlineStr">
         <is>
           <t>ArbeitsmarktRank</t>
         </is>
       </c>
-      <c r="AA1" t="inlineStr">
+      <c r="AB1" t="inlineStr">
         <is>
           <t>BevoelkerungRank</t>
         </is>
       </c>
-      <c r="AB1" t="inlineStr">
+      <c r="AC1" t="inlineStr">
         <is>
           <t>ErreichbarkeitRank</t>
         </is>
       </c>
-      <c r="AC1" t="inlineStr">
+      <c r="AD1" t="inlineStr">
         <is>
           <t>SicherheitRank</t>
         </is>
       </c>
-      <c r="AD1" t="inlineStr">
+      <c r="AE1" t="inlineStr">
         <is>
           <t>SteuernRank</t>
         </is>
       </c>
-      <c r="AE1" t="inlineStr">
+      <c r="AF1" t="inlineStr">
         <is>
           <t>VersorgungRank</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>AuslaenderAnteilRank</t>
         </is>
       </c>
     </row>
@@ -310,25 +320,31 @@
         <v>3.57</v>
       </c>
       <c r="Y2" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="Z2" t="n">
         <v>14.0</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="AA2" t="n">
         <v>29.0</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="AB2" t="n">
         <v>12.0</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="AC2" t="n">
         <v>14.0</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="AD2" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="AE2" t="n">
         <v>47.0</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="AF2" t="n">
         <v>56.0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>38.0</v>
       </c>
     </row>
     <row r="3">
@@ -423,25 +439,31 @@
         <v>1.71</v>
       </c>
       <c r="Y3" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="Z3" t="n">
         <v>20.0</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="AA3" t="n">
         <v>7.0</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="AB3" t="n">
         <v>23.0</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="AC3" t="n">
         <v>44.0</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="AD3" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="AE3" t="n">
         <v>34.0</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="AF3" t="n">
         <v>8.0</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>43.0</v>
       </c>
     </row>
     <row r="4">
@@ -536,25 +558,31 @@
         <v>1.56</v>
       </c>
       <c r="Y4" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="Z4" t="n">
         <v>73.0</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="AA4" t="n">
         <v>57.0</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="AB4" t="n">
         <v>47.0</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="AC4" t="n">
         <v>75.0</v>
       </c>
-      <c r="AC4" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE4" t="n">
         <v>51.0</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="AF4" t="n">
         <v>49.0</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>47.0</v>
       </c>
     </row>
     <row r="5">
@@ -649,25 +677,31 @@
         <v>1.54</v>
       </c>
       <c r="Y5" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="Z5" t="n">
         <v>50.0</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="AA5" t="n">
         <v>58.0</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="AB5" t="n">
         <v>41.0</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="AC5" t="n">
         <v>33.0</v>
       </c>
-      <c r="AC5" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE5" t="n">
         <v>72.0</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="AF5" t="n">
         <v>26.0</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>24.0</v>
       </c>
     </row>
     <row r="6">
@@ -762,25 +796,31 @@
         <v>2.03</v>
       </c>
       <c r="Y6" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="Z6" t="n">
         <v>54.0</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="AA6" t="n">
         <v>51.0</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="AB6" t="n">
         <v>54.0</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="AC6" t="n">
         <v>8.0</v>
       </c>
-      <c r="AC6" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE6" t="n">
         <v>14.0</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="AF6" t="n">
         <v>62.0</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>69.0</v>
       </c>
     </row>
     <row r="7">
@@ -875,25 +915,31 @@
         <v>0.98</v>
       </c>
       <c r="Y7" t="n">
+        <v>9.3</v>
+      </c>
+      <c r="Z7" t="n">
         <v>20.0</v>
       </c>
-      <c r="Z7" t="n">
+      <c r="AA7" t="n">
         <v>7.0</v>
       </c>
-      <c r="AA7" t="n">
+      <c r="AB7" t="n">
         <v>23.0</v>
       </c>
-      <c r="AB7" t="n">
+      <c r="AC7" t="n">
         <v>44.0</v>
       </c>
-      <c r="AC7" t="n">
+      <c r="AD7" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD7" t="n">
+      <c r="AE7" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE7" t="n">
+      <c r="AF7" t="n">
         <v>8.0</v>
+      </c>
+      <c r="AG7" t="n">
+        <v>33.0</v>
       </c>
     </row>
     <row r="8">
@@ -988,25 +1034,31 @@
         <v>1.51</v>
       </c>
       <c r="Y8" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="Z8" t="n">
         <v>10.0</v>
       </c>
-      <c r="Z8" t="n">
+      <c r="AA8" t="n">
         <v>6.0</v>
       </c>
-      <c r="AA8" t="n">
+      <c r="AB8" t="n">
         <v>5.0</v>
       </c>
-      <c r="AB8" t="n">
+      <c r="AC8" t="n">
         <v>26.0</v>
       </c>
-      <c r="AC8" t="n">
+      <c r="AD8" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD8" t="n">
+      <c r="AE8" t="n">
         <v>8.0</v>
       </c>
-      <c r="AE8" t="n">
+      <c r="AF8" t="n">
         <v>52.0</v>
+      </c>
+      <c r="AG8" t="n">
+        <v>17.0</v>
       </c>
     </row>
     <row r="9">
@@ -1101,25 +1153,31 @@
         <v>2.12</v>
       </c>
       <c r="Y9" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="Z9" t="n">
         <v>48.0</v>
       </c>
-      <c r="Z9" t="n">
+      <c r="AA9" t="n">
         <v>61.0</v>
       </c>
-      <c r="AA9" t="n">
+      <c r="AB9" t="n">
         <v>20.0</v>
       </c>
-      <c r="AB9" t="n">
+      <c r="AC9" t="n">
         <v>73.0</v>
       </c>
-      <c r="AC9" t="n">
+      <c r="AD9" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD9" t="n">
+      <c r="AE9" t="n">
         <v>25.0</v>
       </c>
-      <c r="AE9" t="n">
+      <c r="AF9" t="n">
         <v>43.0</v>
+      </c>
+      <c r="AG9" t="n">
+        <v>51.0</v>
       </c>
     </row>
     <row r="10">
@@ -1214,25 +1272,31 @@
         <v>2.12</v>
       </c>
       <c r="Y10" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="Z10" t="n">
         <v>48.0</v>
       </c>
-      <c r="Z10" t="n">
+      <c r="AA10" t="n">
         <v>61.0</v>
       </c>
-      <c r="AA10" t="n">
+      <c r="AB10" t="n">
         <v>20.0</v>
       </c>
-      <c r="AB10" t="n">
+      <c r="AC10" t="n">
         <v>73.0</v>
       </c>
-      <c r="AC10" t="n">
+      <c r="AD10" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD10" t="n">
+      <c r="AE10" t="n">
         <v>25.0</v>
       </c>
-      <c r="AE10" t="n">
+      <c r="AF10" t="n">
         <v>43.0</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>51.0</v>
       </c>
     </row>
     <row r="11">
@@ -1327,25 +1391,31 @@
         <v>1.93</v>
       </c>
       <c r="Y11" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="Z11" t="n">
         <v>18.0</v>
       </c>
-      <c r="Z11" t="n">
+      <c r="AA11" t="n">
         <v>21.0</v>
       </c>
-      <c r="AA11" t="n">
+      <c r="AB11" t="n">
         <v>62.0</v>
       </c>
-      <c r="AB11" t="n">
+      <c r="AC11" t="n">
         <v>21.0</v>
       </c>
-      <c r="AC11" t="n">
+      <c r="AD11" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD11" t="n">
+      <c r="AE11" t="n">
         <v>34.0</v>
       </c>
-      <c r="AE11" t="n">
+      <c r="AF11" t="n">
         <v>86.0</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>72.0</v>
       </c>
     </row>
     <row r="12">
@@ -1440,25 +1510,31 @@
         <v>1.89</v>
       </c>
       <c r="Y12" t="n">
+        <v>12.1</v>
+      </c>
+      <c r="Z12" t="n">
         <v>83.0</v>
       </c>
-      <c r="Z12" t="n">
+      <c r="AA12" t="n">
         <v>81.0</v>
       </c>
-      <c r="AA12" t="n">
+      <c r="AB12" t="n">
         <v>58.0</v>
       </c>
-      <c r="AB12" t="n">
+      <c r="AC12" t="n">
         <v>82.0</v>
       </c>
-      <c r="AC12" t="n">
+      <c r="AD12" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD12" t="n">
+      <c r="AE12" t="n">
         <v>47.0</v>
       </c>
-      <c r="AE12" t="n">
+      <c r="AF12" t="n">
         <v>72.0</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>53.0</v>
       </c>
     </row>
     <row r="13">
@@ -1553,25 +1629,31 @@
         <v>2.06</v>
       </c>
       <c r="Y13" t="n">
+        <v>25.2</v>
+      </c>
+      <c r="Z13" t="n">
         <v>87.0</v>
       </c>
-      <c r="Z13" t="n">
+      <c r="AA13" t="n">
         <v>85.0</v>
       </c>
-      <c r="AA13" t="n">
+      <c r="AB13" t="n">
         <v>66.0</v>
       </c>
-      <c r="AB13" t="n">
+      <c r="AC13" t="n">
         <v>58.0</v>
       </c>
-      <c r="AC13" t="n">
+      <c r="AD13" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD13" t="n">
+      <c r="AE13" t="n">
         <v>72.0</v>
       </c>
-      <c r="AE13" t="n">
+      <c r="AF13" t="n">
         <v>55.0</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>85.0</v>
       </c>
     </row>
     <row r="14">
@@ -1666,25 +1748,31 @@
         <v>1.33</v>
       </c>
       <c r="Y14" t="n">
+        <v>14.2</v>
+      </c>
+      <c r="Z14" t="n">
         <v>35.0</v>
       </c>
-      <c r="Z14" t="n">
+      <c r="AA14" t="n">
         <v>22.0</v>
       </c>
-      <c r="AA14" t="n">
+      <c r="AB14" t="n">
         <v>50.0</v>
       </c>
-      <c r="AB14" t="n">
+      <c r="AC14" t="n">
         <v>9.0</v>
       </c>
-      <c r="AC14" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD14" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE14" t="n">
         <v>25.0</v>
       </c>
-      <c r="AE14" t="n">
+      <c r="AF14" t="n">
         <v>88.0</v>
+      </c>
+      <c r="AG14" t="n">
+        <v>58.0</v>
       </c>
     </row>
     <row r="15">
@@ -1779,25 +1867,31 @@
         <v>1.53</v>
       </c>
       <c r="Y15" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="Z15" t="n">
         <v>20.0</v>
       </c>
-      <c r="Z15" t="n">
+      <c r="AA15" t="n">
         <v>26.0</v>
       </c>
-      <c r="AA15" t="n">
+      <c r="AB15" t="n">
         <v>38.0</v>
       </c>
-      <c r="AB15" t="n">
+      <c r="AC15" t="n">
         <v>10.0</v>
       </c>
-      <c r="AC15" t="n">
+      <c r="AD15" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD15" t="n">
+      <c r="AE15" t="n">
         <v>25.0</v>
       </c>
-      <c r="AE15" t="n">
+      <c r="AF15" t="n">
         <v>60.0</v>
+      </c>
+      <c r="AG15" t="n">
+        <v>66.0</v>
       </c>
     </row>
     <row r="16">
@@ -1892,25 +1986,31 @@
         <v>0.94</v>
       </c>
       <c r="Y16" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="Z16" t="n">
         <v>66.0</v>
       </c>
-      <c r="Z16" t="n">
+      <c r="AA16" t="n">
         <v>70.0</v>
       </c>
-      <c r="AA16" t="n">
+      <c r="AB16" t="n">
         <v>79.0</v>
       </c>
-      <c r="AB16" t="n">
+      <c r="AC16" t="n">
         <v>61.0</v>
       </c>
-      <c r="AC16" t="n">
+      <c r="AD16" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD16" t="n">
+      <c r="AE16" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE16" t="n">
+      <c r="AF16" t="n">
         <v>74.0</v>
+      </c>
+      <c r="AG16" t="n">
+        <v>4.0</v>
       </c>
     </row>
     <row r="17">
@@ -2005,25 +2105,31 @@
         <v>2.0</v>
       </c>
       <c r="Y17" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="Z17" t="n">
         <v>69.0</v>
       </c>
-      <c r="Z17" t="n">
+      <c r="AA17" t="n">
         <v>72.0</v>
       </c>
-      <c r="AA17" t="n">
+      <c r="AB17" t="n">
         <v>48.0</v>
       </c>
-      <c r="AB17" t="n">
+      <c r="AC17" t="n">
         <v>17.0</v>
       </c>
-      <c r="AC17" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD17" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE17" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE17" t="n">
+      <c r="AF17" t="n">
         <v>59.0</v>
+      </c>
+      <c r="AG17" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="18">
@@ -2118,25 +2224,31 @@
         <v>1.44</v>
       </c>
       <c r="Y18" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="Z18" t="n">
         <v>30.0</v>
       </c>
-      <c r="Z18" t="n">
+      <c r="AA18" t="n">
         <v>34.0</v>
       </c>
-      <c r="AA18" t="n">
+      <c r="AB18" t="n">
         <v>60.0</v>
       </c>
-      <c r="AB18" t="n">
+      <c r="AC18" t="n">
         <v>4.0</v>
       </c>
-      <c r="AC18" t="n">
+      <c r="AD18" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD18" t="n">
+      <c r="AE18" t="n">
         <v>18.0</v>
       </c>
-      <c r="AE18" t="n">
+      <c r="AF18" t="n">
         <v>73.0</v>
+      </c>
+      <c r="AG18" t="n">
+        <v>76.0</v>
       </c>
     </row>
     <row r="19">
@@ -2231,25 +2343,31 @@
         <v>1.97</v>
       </c>
       <c r="Y19" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="Z19" t="n">
         <v>53.0</v>
       </c>
-      <c r="Z19" t="n">
+      <c r="AA19" t="n">
         <v>46.0</v>
       </c>
-      <c r="AA19" t="n">
+      <c r="AB19" t="n">
         <v>40.0</v>
       </c>
-      <c r="AB19" t="n">
+      <c r="AC19" t="n">
         <v>23.0</v>
       </c>
-      <c r="AC19" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD19" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE19" t="n">
         <v>34.0</v>
       </c>
-      <c r="AE19" t="n">
+      <c r="AF19" t="n">
         <v>83.0</v>
+      </c>
+      <c r="AG19" t="n">
+        <v>28.0</v>
       </c>
     </row>
     <row r="20">
@@ -2344,25 +2462,31 @@
         <v>3.22</v>
       </c>
       <c r="Y20" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="Z20" t="n">
         <v>16.0</v>
       </c>
-      <c r="Z20" t="n">
+      <c r="AA20" t="n">
         <v>23.0</v>
       </c>
-      <c r="AA20" t="n">
+      <c r="AB20" t="n">
         <v>11.0</v>
       </c>
-      <c r="AB20" t="n">
+      <c r="AC20" t="n">
         <v>42.0</v>
       </c>
-      <c r="AC20" t="n">
+      <c r="AD20" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD20" t="n">
+      <c r="AE20" t="n">
         <v>4.0</v>
       </c>
-      <c r="AE20" t="n">
+      <c r="AF20" t="n">
         <v>32.0</v>
+      </c>
+      <c r="AG20" t="n">
+        <v>17.0</v>
       </c>
     </row>
     <row r="21">
@@ -2457,25 +2581,31 @@
         <v>1.32</v>
       </c>
       <c r="Y21" t="n">
+        <v>33.3</v>
+      </c>
+      <c r="Z21" t="n">
         <v>28.0</v>
       </c>
-      <c r="Z21" t="n">
+      <c r="AA21" t="n">
         <v>27.0</v>
       </c>
-      <c r="AA21" t="n">
+      <c r="AB21" t="n">
         <v>88.0</v>
       </c>
-      <c r="AB21" t="n">
+      <c r="AC21" t="n">
         <v>15.0</v>
       </c>
-      <c r="AC21" t="n">
+      <c r="AD21" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD21" t="n">
+      <c r="AE21" t="n">
         <v>65.0</v>
       </c>
-      <c r="AE21" t="n">
+      <c r="AF21" t="n">
         <v>38.0</v>
+      </c>
+      <c r="AG21" t="n">
+        <v>88.0</v>
       </c>
     </row>
     <row r="22">
@@ -2570,25 +2700,31 @@
         <v>1.14</v>
       </c>
       <c r="Y22" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="Z22" t="n">
         <v>69.0</v>
       </c>
-      <c r="Z22" t="n">
+      <c r="AA22" t="n">
         <v>76.0</v>
       </c>
-      <c r="AA22" t="n">
+      <c r="AB22" t="n">
         <v>73.0</v>
       </c>
-      <c r="AB22" t="n">
+      <c r="AC22" t="n">
         <v>70.0</v>
       </c>
-      <c r="AC22" t="n">
+      <c r="AD22" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD22" t="n">
+      <c r="AE22" t="n">
         <v>57.0</v>
       </c>
-      <c r="AE22" t="n">
+      <c r="AF22" t="n">
         <v>84.0</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>20.0</v>
       </c>
     </row>
     <row r="23">
@@ -2683,25 +2819,31 @@
         <v>2.08</v>
       </c>
       <c r="Y23" t="n">
+        <v>11.3</v>
+      </c>
+      <c r="Z23" t="n">
         <v>37.0</v>
       </c>
-      <c r="Z23" t="n">
+      <c r="AA23" t="n">
         <v>31.0</v>
       </c>
-      <c r="AA23" t="n">
+      <c r="AB23" t="n">
         <v>22.0</v>
       </c>
-      <c r="AB23" t="n">
+      <c r="AC23" t="n">
         <v>60.0</v>
-      </c>
-      <c r="AC23" t="n">
-        <v>57.0</v>
       </c>
       <c r="AD23" t="n">
         <v>57.0</v>
       </c>
       <c r="AE23" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="AF23" t="n">
         <v>21.0</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>46.0</v>
       </c>
     </row>
     <row r="24">
@@ -2796,25 +2938,31 @@
         <v>2.39</v>
       </c>
       <c r="Y24" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="Z24" t="n">
         <v>29.0</v>
       </c>
-      <c r="Z24" t="n">
+      <c r="AA24" t="n">
         <v>44.0</v>
       </c>
-      <c r="AA24" t="n">
+      <c r="AB24" t="n">
         <v>16.0</v>
       </c>
-      <c r="AB24" t="n">
+      <c r="AC24" t="n">
         <v>27.0</v>
       </c>
-      <c r="AC24" t="n">
+      <c r="AD24" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD24" t="n">
+      <c r="AE24" t="n">
         <v>6.0</v>
       </c>
-      <c r="AE24" t="n">
+      <c r="AF24" t="n">
         <v>87.0</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>40.0</v>
       </c>
     </row>
     <row r="25">
@@ -2909,24 +3057,30 @@
         <v>1.09</v>
       </c>
       <c r="Y25" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="Z25" t="n">
         <v>84.0</v>
       </c>
-      <c r="Z25" t="n">
+      <c r="AA25" t="n">
         <v>86.0</v>
       </c>
-      <c r="AA25" t="n">
+      <c r="AB25" t="n">
         <v>85.0</v>
       </c>
-      <c r="AB25" t="n">
+      <c r="AC25" t="n">
         <v>76.0</v>
       </c>
-      <c r="AC25" t="n">
+      <c r="AD25" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD25" t="n">
+      <c r="AE25" t="n">
         <v>42.0</v>
       </c>
-      <c r="AE25" t="n">
+      <c r="AF25" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="AG25" t="n">
         <v>12.0</v>
       </c>
     </row>
@@ -3022,24 +3176,30 @@
         <v>1.09</v>
       </c>
       <c r="Y26" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="Z26" t="n">
         <v>84.0</v>
       </c>
-      <c r="Z26" t="n">
+      <c r="AA26" t="n">
         <v>86.0</v>
       </c>
-      <c r="AA26" t="n">
+      <c r="AB26" t="n">
         <v>85.0</v>
       </c>
-      <c r="AB26" t="n">
+      <c r="AC26" t="n">
         <v>76.0</v>
       </c>
-      <c r="AC26" t="n">
+      <c r="AD26" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD26" t="n">
+      <c r="AE26" t="n">
         <v>42.0</v>
       </c>
-      <c r="AE26" t="n">
+      <c r="AF26" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="AG26" t="n">
         <v>12.0</v>
       </c>
     </row>
@@ -3135,24 +3295,30 @@
         <v>1.09</v>
       </c>
       <c r="Y27" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="Z27" t="n">
         <v>84.0</v>
       </c>
-      <c r="Z27" t="n">
+      <c r="AA27" t="n">
         <v>86.0</v>
       </c>
-      <c r="AA27" t="n">
+      <c r="AB27" t="n">
         <v>85.0</v>
       </c>
-      <c r="AB27" t="n">
+      <c r="AC27" t="n">
         <v>76.0</v>
       </c>
-      <c r="AC27" t="n">
+      <c r="AD27" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD27" t="n">
+      <c r="AE27" t="n">
         <v>42.0</v>
       </c>
-      <c r="AE27" t="n">
+      <c r="AF27" t="n">
+        <v>12.0</v>
+      </c>
+      <c r="AG27" t="n">
         <v>12.0</v>
       </c>
     </row>
@@ -3248,25 +3414,31 @@
         <v>1.56</v>
       </c>
       <c r="Y28" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="Z28" t="n">
         <v>81.0</v>
       </c>
-      <c r="Z28" t="n">
+      <c r="AA28" t="n">
         <v>52.0</v>
       </c>
-      <c r="AA28" t="n">
+      <c r="AB28" t="n">
         <v>44.0</v>
       </c>
-      <c r="AB28" t="n">
+      <c r="AC28" t="n">
         <v>79.0</v>
       </c>
-      <c r="AC28" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD28" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE28" t="n">
         <v>51.0</v>
       </c>
-      <c r="AE28" t="n">
+      <c r="AF28" t="n">
         <v>63.0</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>27.0</v>
       </c>
     </row>
     <row r="29">
@@ -3361,25 +3533,31 @@
         <v>1.64</v>
       </c>
       <c r="Y29" t="n">
+        <v>10.1</v>
+      </c>
+      <c r="Z29" t="n">
         <v>75.0</v>
       </c>
-      <c r="Z29" t="n">
+      <c r="AA29" t="n">
         <v>68.0</v>
       </c>
-      <c r="AA29" t="n">
+      <c r="AB29" t="n">
         <v>53.0</v>
       </c>
-      <c r="AB29" t="n">
+      <c r="AC29" t="n">
         <v>56.0</v>
       </c>
-      <c r="AC29" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD29" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE29" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE29" t="n">
+      <c r="AF29" t="n">
         <v>57.0</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>39.0</v>
       </c>
     </row>
     <row r="30">
@@ -3474,25 +3652,31 @@
         <v>1.22</v>
       </c>
       <c r="Y30" t="n">
+        <v>17.3</v>
+      </c>
+      <c r="Z30" t="n">
         <v>57.0</v>
       </c>
-      <c r="Z30" t="n">
+      <c r="AA30" t="n">
         <v>53.0</v>
       </c>
-      <c r="AA30" t="n">
+      <c r="AB30" t="n">
         <v>78.0</v>
       </c>
-      <c r="AB30" t="n">
+      <c r="AC30" t="n">
         <v>72.0</v>
       </c>
-      <c r="AC30" t="n">
+      <c r="AD30" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD30" t="n">
+      <c r="AE30" t="n">
         <v>34.0</v>
       </c>
-      <c r="AE30" t="n">
+      <c r="AF30" t="n">
         <v>31.0</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>68.0</v>
       </c>
     </row>
     <row r="31">
@@ -3587,25 +3771,31 @@
         <v>1.1</v>
       </c>
       <c r="Y31" t="n">
+        <v>19.2</v>
+      </c>
+      <c r="Z31" t="n">
         <v>72.0</v>
       </c>
-      <c r="Z31" t="n">
+      <c r="AA31" t="n">
         <v>66.0</v>
       </c>
-      <c r="AA31" t="n">
+      <c r="AB31" t="n">
         <v>56.0</v>
       </c>
-      <c r="AB31" t="n">
+      <c r="AC31" t="n">
         <v>70.0</v>
       </c>
-      <c r="AC31" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD31" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE31" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE31" t="n">
+      <c r="AF31" t="n">
         <v>39.0</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>75.0</v>
       </c>
     </row>
     <row r="32">
@@ -3700,25 +3890,31 @@
         <v>1.71</v>
       </c>
       <c r="Y32" t="n">
+        <v>21.1</v>
+      </c>
+      <c r="Z32" t="n">
         <v>43.0</v>
       </c>
-      <c r="Z32" t="n">
+      <c r="AA32" t="n">
         <v>32.0</v>
       </c>
-      <c r="AA32" t="n">
+      <c r="AB32" t="n">
         <v>17.0</v>
       </c>
-      <c r="AB32" t="n">
+      <c r="AC32" t="n">
         <v>44.0</v>
       </c>
-      <c r="AC32" t="n">
+      <c r="AD32" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD32" t="n">
+      <c r="AE32" t="n">
         <v>72.0</v>
       </c>
-      <c r="AE32" t="n">
+      <c r="AF32" t="n">
         <v>77.0</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>78.0</v>
       </c>
     </row>
     <row r="33">
@@ -3813,25 +4009,31 @@
         <v>1.94</v>
       </c>
       <c r="Y33" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="Z33" t="n">
         <v>40.0</v>
       </c>
-      <c r="Z33" t="n">
+      <c r="AA33" t="n">
         <v>42.0</v>
       </c>
-      <c r="AA33" t="n">
+      <c r="AB33" t="n">
         <v>51.0</v>
       </c>
-      <c r="AB33" t="n">
+      <c r="AC33" t="n">
         <v>18.0</v>
       </c>
-      <c r="AC33" t="n">
+      <c r="AD33" t="n">
         <v>73.0</v>
       </c>
-      <c r="AD33" t="n">
+      <c r="AE33" t="n">
         <v>10.0</v>
       </c>
-      <c r="AE33" t="n">
+      <c r="AF33" t="n">
         <v>41.0</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>70.0</v>
       </c>
     </row>
     <row r="34">
@@ -3926,25 +4128,31 @@
         <v>1.06</v>
       </c>
       <c r="Y34" t="n">
+        <v>16.7</v>
+      </c>
+      <c r="Z34" t="n">
         <v>6.0</v>
       </c>
-      <c r="Z34" t="n">
+      <c r="AA34" t="n">
         <v>35.0</v>
       </c>
-      <c r="AA34" t="n">
+      <c r="AB34" t="n">
         <v>13.0</v>
       </c>
-      <c r="AB34" t="n">
+      <c r="AC34" t="n">
         <v>51.0</v>
       </c>
-      <c r="AC34" t="n">
+      <c r="AD34" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD34" t="n">
+      <c r="AE34" t="n">
         <v>25.0</v>
       </c>
-      <c r="AE34" t="n">
-        <v>1.0</v>
+      <c r="AF34" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>65.0</v>
       </c>
     </row>
     <row r="35">
@@ -4039,25 +4247,31 @@
         <v>2.39</v>
       </c>
       <c r="Y35" t="n">
+        <v>6.9</v>
+      </c>
+      <c r="Z35" t="n">
         <v>60.0</v>
       </c>
-      <c r="Z35" t="n">
+      <c r="AA35" t="n">
         <v>67.0</v>
       </c>
-      <c r="AA35" t="n">
+      <c r="AB35" t="n">
         <v>49.0</v>
       </c>
-      <c r="AB35" t="n">
+      <c r="AC35" t="n">
         <v>28.0</v>
       </c>
-      <c r="AC35" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD35" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE35" t="n">
         <v>72.0</v>
       </c>
-      <c r="AE35" t="n">
+      <c r="AF35" t="n">
         <v>47.0</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>21.0</v>
       </c>
     </row>
     <row r="36">
@@ -4152,25 +4366,31 @@
         <v>1.64</v>
       </c>
       <c r="Y36" t="n">
+        <v>12.3</v>
+      </c>
+      <c r="Z36" t="n">
         <v>47.0</v>
       </c>
-      <c r="Z36" t="n">
+      <c r="AA36" t="n">
         <v>48.0</v>
       </c>
-      <c r="AA36" t="n">
+      <c r="AB36" t="n">
         <v>57.0</v>
       </c>
-      <c r="AB36" t="n">
+      <c r="AC36" t="n">
         <v>84.0</v>
       </c>
-      <c r="AC36" t="n">
+      <c r="AD36" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD36" t="n">
+      <c r="AE36" t="n">
         <v>25.0</v>
       </c>
-      <c r="AE36" t="n">
+      <c r="AF36" t="n">
         <v>85.0</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>54.0</v>
       </c>
     </row>
     <row r="37">
@@ -4265,25 +4485,31 @@
         <v>1.57</v>
       </c>
       <c r="Y37" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="Z37" t="n">
         <v>55.0</v>
       </c>
-      <c r="Z37" t="n">
+      <c r="AA37" t="n">
         <v>49.0</v>
       </c>
-      <c r="AA37" t="n">
+      <c r="AB37" t="n">
         <v>71.0</v>
       </c>
-      <c r="AB37" t="n">
+      <c r="AC37" t="n">
         <v>68.0</v>
       </c>
-      <c r="AC37" t="n">
+      <c r="AD37" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD37" t="n">
+      <c r="AE37" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE37" t="n">
+      <c r="AF37" t="n">
         <v>76.0</v>
+      </c>
+      <c r="AG37" t="n">
+        <v>4.0</v>
       </c>
     </row>
     <row r="38">
@@ -4378,25 +4604,31 @@
         <v>0.75</v>
       </c>
       <c r="Y38" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="Z38" t="n">
         <v>82.0</v>
       </c>
-      <c r="Z38" t="n">
+      <c r="AA38" t="n">
         <v>77.0</v>
       </c>
-      <c r="AA38" t="n">
+      <c r="AB38" t="n">
         <v>72.0</v>
       </c>
-      <c r="AB38" t="n">
+      <c r="AC38" t="n">
         <v>86.0</v>
       </c>
-      <c r="AC38" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD38" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE38" t="n">
         <v>57.0</v>
       </c>
-      <c r="AE38" t="n">
+      <c r="AF38" t="n">
         <v>35.0</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>12.0</v>
       </c>
     </row>
     <row r="39">
@@ -4491,25 +4723,31 @@
         <v>2.0</v>
       </c>
       <c r="Y39" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="Z39" t="n">
         <v>9.0</v>
       </c>
-      <c r="Z39" t="n">
+      <c r="AA39" t="n">
         <v>14.0</v>
       </c>
-      <c r="AA39" t="n">
+      <c r="AB39" t="n">
         <v>3.0</v>
       </c>
-      <c r="AB39" t="n">
+      <c r="AC39" t="n">
         <v>38.0</v>
       </c>
-      <c r="AC39" t="n">
+      <c r="AD39" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD39" t="n">
+      <c r="AE39" t="n">
         <v>11.0</v>
       </c>
-      <c r="AE39" t="n">
+      <c r="AF39" t="n">
         <v>60.0</v>
+      </c>
+      <c r="AG39" t="n">
+        <v>24.0</v>
       </c>
     </row>
     <row r="40">
@@ -4604,25 +4842,31 @@
         <v>2.29</v>
       </c>
       <c r="Y40" t="n">
+        <v>14.8</v>
+      </c>
+      <c r="Z40" t="n">
         <v>20.0</v>
       </c>
-      <c r="Z40" t="n">
+      <c r="AA40" t="n">
         <v>7.0</v>
       </c>
-      <c r="AA40" t="n">
+      <c r="AB40" t="n">
         <v>23.0</v>
       </c>
-      <c r="AB40" t="n">
+      <c r="AC40" t="n">
         <v>44.0</v>
       </c>
-      <c r="AC40" t="n">
+      <c r="AD40" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD40" t="n">
+      <c r="AE40" t="n">
         <v>42.0</v>
       </c>
-      <c r="AE40" t="n">
+      <c r="AF40" t="n">
         <v>8.0</v>
+      </c>
+      <c r="AG40" t="n">
+        <v>59.0</v>
       </c>
     </row>
     <row r="41">
@@ -4717,25 +4961,31 @@
         <v>1.7</v>
       </c>
       <c r="Y41" t="n">
+        <v>20.9</v>
+      </c>
+      <c r="Z41" t="n">
         <v>34.0</v>
       </c>
-      <c r="Z41" t="n">
+      <c r="AA41" t="n">
         <v>19.0</v>
       </c>
-      <c r="AA41" t="n">
+      <c r="AB41" t="n">
         <v>45.0</v>
       </c>
-      <c r="AB41" t="n">
+      <c r="AC41" t="n">
         <v>39.0</v>
       </c>
-      <c r="AC41" t="n">
+      <c r="AD41" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD41" t="n">
+      <c r="AE41" t="n">
         <v>47.0</v>
       </c>
-      <c r="AE41" t="n">
+      <c r="AF41" t="n">
         <v>17.0</v>
+      </c>
+      <c r="AG41" t="n">
+        <v>77.0</v>
       </c>
     </row>
     <row r="42">
@@ -4830,25 +5080,31 @@
         <v>2.46</v>
       </c>
       <c r="Y42" t="n">
+        <v>6.6</v>
+      </c>
+      <c r="Z42" t="n">
         <v>71.0</v>
       </c>
-      <c r="Z42" t="n">
+      <c r="AA42" t="n">
         <v>80.0</v>
       </c>
-      <c r="AA42" t="n">
+      <c r="AB42" t="n">
         <v>33.0</v>
       </c>
-      <c r="AB42" t="n">
+      <c r="AC42" t="n">
         <v>68.0</v>
       </c>
-      <c r="AC42" t="n">
+      <c r="AD42" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD42" t="n">
+      <c r="AE42" t="n">
         <v>65.0</v>
       </c>
-      <c r="AE42" t="n">
+      <c r="AF42" t="n">
         <v>81.0</v>
+      </c>
+      <c r="AG42" t="n">
+        <v>19.0</v>
       </c>
     </row>
     <row r="43">
@@ -4943,25 +5199,31 @@
         <v>2.89</v>
       </c>
       <c r="Y43" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="Z43" t="n">
         <v>44.0</v>
       </c>
-      <c r="Z43" t="n">
+      <c r="AA43" t="n">
         <v>39.0</v>
       </c>
-      <c r="AA43" t="n">
+      <c r="AB43" t="n">
         <v>29.0</v>
       </c>
-      <c r="AB43" t="n">
+      <c r="AC43" t="n">
         <v>30.0</v>
       </c>
-      <c r="AC43" t="n">
+      <c r="AD43" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD43" t="n">
+      <c r="AE43" t="n">
         <v>18.0</v>
       </c>
-      <c r="AE43" t="n">
+      <c r="AF43" t="n">
         <v>53.0</v>
+      </c>
+      <c r="AG43" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="44">
@@ -5056,25 +5318,31 @@
         <v>2.42</v>
       </c>
       <c r="Y44" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="Z44" t="n">
         <v>2.0</v>
       </c>
-      <c r="Z44" t="n">
+      <c r="AA44" t="n">
         <v>4.0</v>
       </c>
-      <c r="AA44" t="n">
+      <c r="AB44" t="n">
         <v>46.0</v>
       </c>
-      <c r="AB44" t="n">
+      <c r="AC44" t="n">
         <v>13.0</v>
       </c>
-      <c r="AC44" t="n">
+      <c r="AD44" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD44" t="n">
+      <c r="AE44" t="n">
         <v>7.0</v>
       </c>
-      <c r="AE44" t="n">
+      <c r="AF44" t="n">
         <v>25.0</v>
+      </c>
+      <c r="AG44" t="n">
+        <v>67.0</v>
       </c>
     </row>
     <row r="45">
@@ -5169,25 +5437,31 @@
         <v>1.36</v>
       </c>
       <c r="Y45" t="n">
+        <v>10.3</v>
+      </c>
+      <c r="Z45" t="n">
         <v>44.0</v>
       </c>
-      <c r="Z45" t="n">
+      <c r="AA45" t="n">
         <v>39.0</v>
       </c>
-      <c r="AA45" t="n">
+      <c r="AB45" t="n">
         <v>29.0</v>
       </c>
-      <c r="AB45" t="n">
+      <c r="AC45" t="n">
         <v>30.0</v>
       </c>
-      <c r="AC45" t="n">
+      <c r="AD45" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD45" t="n">
+      <c r="AE45" t="n">
         <v>18.0</v>
       </c>
-      <c r="AE45" t="n">
+      <c r="AF45" t="n">
         <v>53.0</v>
+      </c>
+      <c r="AG45" t="n">
+        <v>42.0</v>
       </c>
     </row>
     <row r="46">
@@ -5282,25 +5556,31 @@
         <v>2.59</v>
       </c>
       <c r="Y46" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="Z46" t="n">
         <v>31.0</v>
       </c>
-      <c r="Z46" t="n">
+      <c r="AA46" t="n">
         <v>41.0</v>
       </c>
-      <c r="AA46" t="n">
+      <c r="AB46" t="n">
         <v>8.0</v>
       </c>
-      <c r="AB46" t="n">
+      <c r="AC46" t="n">
         <v>55.0</v>
       </c>
-      <c r="AC46" t="n">
+      <c r="AD46" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD46" t="n">
+      <c r="AE46" t="n">
         <v>51.0</v>
       </c>
-      <c r="AE46" t="n">
+      <c r="AF46" t="n">
         <v>40.0</v>
+      </c>
+      <c r="AG46" t="n">
+        <v>35.0</v>
       </c>
     </row>
     <row r="47">
@@ -5395,25 +5675,31 @@
         <v>1.99</v>
       </c>
       <c r="Y47" t="n">
+        <v>17.7</v>
+      </c>
+      <c r="Z47" t="n">
         <v>36.0</v>
       </c>
-      <c r="Z47" t="n">
+      <c r="AA47" t="n">
         <v>38.0</v>
       </c>
-      <c r="AA47" t="n">
+      <c r="AB47" t="n">
         <v>83.0</v>
       </c>
-      <c r="AB47" t="n">
+      <c r="AC47" t="n">
         <v>5.0</v>
       </c>
-      <c r="AC47" t="n">
+      <c r="AD47" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD47" t="n">
+      <c r="AE47" t="n">
         <v>34.0</v>
       </c>
-      <c r="AE47" t="n">
+      <c r="AF47" t="n">
         <v>42.0</v>
+      </c>
+      <c r="AG47" t="n">
+        <v>71.0</v>
       </c>
     </row>
     <row r="48">
@@ -5508,25 +5794,31 @@
         <v>0.84</v>
       </c>
       <c r="Y48" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="Z48" t="n">
         <v>58.0</v>
-      </c>
-      <c r="Z48" t="n">
-        <v>63.0</v>
       </c>
       <c r="AA48" t="n">
         <v>63.0</v>
       </c>
       <c r="AB48" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="AC48" t="n">
         <v>87.0</v>
       </c>
-      <c r="AC48" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD48" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE48" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE48" t="n">
+      <c r="AF48" t="n">
         <v>15.0</v>
+      </c>
+      <c r="AG48" t="n">
+        <v>7.0</v>
       </c>
     </row>
     <row r="49">
@@ -5621,25 +5913,31 @@
         <v>1.45</v>
       </c>
       <c r="Y49" t="n">
+        <v>24.2</v>
+      </c>
+      <c r="Z49" t="n">
         <v>4.0</v>
       </c>
-      <c r="Z49" t="n">
+      <c r="AA49" t="n">
         <v>18.0</v>
       </c>
-      <c r="AA49" t="n">
+      <c r="AB49" t="n">
         <v>74.0</v>
       </c>
-      <c r="AB49" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AC49" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AD49" t="n">
         <v>88.0</v>
       </c>
-      <c r="AD49" t="n">
+      <c r="AE49" t="n">
         <v>16.0</v>
       </c>
-      <c r="AE49" t="n">
+      <c r="AF49" t="n">
         <v>7.0</v>
+      </c>
+      <c r="AG49" t="n">
+        <v>82.0</v>
       </c>
     </row>
     <row r="50">
@@ -5734,25 +6032,31 @@
         <v>1.81</v>
       </c>
       <c r="Y50" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="Z50" t="n">
         <v>33.0</v>
       </c>
-      <c r="Z50" t="n">
+      <c r="AA50" t="n">
         <v>24.0</v>
       </c>
-      <c r="AA50" t="n">
+      <c r="AB50" t="n">
         <v>68.0</v>
       </c>
-      <c r="AB50" t="n">
+      <c r="AC50" t="n">
         <v>20.0</v>
       </c>
-      <c r="AC50" t="n">
+      <c r="AD50" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD50" t="n">
+      <c r="AE50" t="n">
         <v>42.0</v>
       </c>
-      <c r="AE50" t="n">
+      <c r="AF50" t="n">
         <v>19.0</v>
+      </c>
+      <c r="AG50" t="n">
+        <v>47.0</v>
       </c>
     </row>
     <row r="51">
@@ -5847,25 +6151,31 @@
         <v>4.01</v>
       </c>
       <c r="Y51" t="n">
+        <v>9.2</v>
+      </c>
+      <c r="Z51" t="n">
         <v>39.0</v>
       </c>
-      <c r="Z51" t="n">
+      <c r="AA51" t="n">
         <v>33.0</v>
       </c>
-      <c r="AA51" t="n">
+      <c r="AB51" t="n">
         <v>37.0</v>
-      </c>
-      <c r="AB51" t="n">
-        <v>36.0</v>
       </c>
       <c r="AC51" t="n">
         <v>36.0</v>
       </c>
       <c r="AD51" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="AE51" t="n">
         <v>47.0</v>
       </c>
-      <c r="AE51" t="n">
+      <c r="AF51" t="n">
         <v>51.0</v>
+      </c>
+      <c r="AG51" t="n">
+        <v>32.0</v>
       </c>
     </row>
     <row r="52">
@@ -5960,25 +6270,31 @@
         <v>3.07</v>
       </c>
       <c r="Y52" t="n">
-        <v>1.0</v>
+        <v>13.8</v>
       </c>
       <c r="Z52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AA52" t="n">
         <v>3.0</v>
       </c>
-      <c r="AA52" t="n">
+      <c r="AB52" t="n">
         <v>6.0</v>
       </c>
-      <c r="AB52" t="n">
+      <c r="AC52" t="n">
         <v>7.0</v>
       </c>
-      <c r="AC52" t="n">
+      <c r="AD52" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD52" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AE52" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AF52" t="n">
         <v>5.0</v>
+      </c>
+      <c r="AG52" t="n">
+        <v>57.0</v>
       </c>
     </row>
     <row r="53">
@@ -6073,25 +6389,31 @@
         <v>0.59</v>
       </c>
       <c r="Y53" t="n">
+        <v>13.6</v>
+      </c>
+      <c r="Z53" t="n">
         <v>27.0</v>
       </c>
-      <c r="Z53" t="n">
+      <c r="AA53" t="n">
         <v>25.0</v>
       </c>
-      <c r="AA53" t="n">
+      <c r="AB53" t="n">
         <v>36.0</v>
       </c>
-      <c r="AB53" t="n">
+      <c r="AC53" t="n">
         <v>12.0</v>
       </c>
-      <c r="AC53" t="n">
+      <c r="AD53" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD53" t="n">
+      <c r="AE53" t="n">
         <v>65.0</v>
       </c>
-      <c r="AE53" t="n">
+      <c r="AF53" t="n">
         <v>43.0</v>
+      </c>
+      <c r="AG53" t="n">
+        <v>56.0</v>
       </c>
     </row>
     <row r="54">
@@ -6186,25 +6508,31 @@
         <v>0.99</v>
       </c>
       <c r="Y54" t="n">
+        <v>9.3</v>
+      </c>
+      <c r="Z54" t="n">
         <v>88.0</v>
       </c>
-      <c r="Z54" t="n">
+      <c r="AA54" t="n">
         <v>84.0</v>
       </c>
-      <c r="AA54" t="n">
+      <c r="AB54" t="n">
         <v>82.0</v>
       </c>
-      <c r="AB54" t="n">
+      <c r="AC54" t="n">
         <v>85.0</v>
       </c>
-      <c r="AC54" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD54" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE54" t="n">
         <v>72.0</v>
       </c>
-      <c r="AE54" t="n">
+      <c r="AF54" t="n">
         <v>64.0</v>
+      </c>
+      <c r="AG54" t="n">
+        <v>33.0</v>
       </c>
     </row>
     <row r="55">
@@ -6299,25 +6627,31 @@
         <v>0.91</v>
       </c>
       <c r="Y55" t="n">
+        <v>26.5</v>
+      </c>
+      <c r="Z55" t="n">
         <v>68.0</v>
       </c>
-      <c r="Z55" t="n">
+      <c r="AA55" t="n">
         <v>72.0</v>
       </c>
-      <c r="AA55" t="n">
+      <c r="AB55" t="n">
         <v>28.0</v>
       </c>
-      <c r="AB55" t="n">
+      <c r="AC55" t="n">
         <v>19.0</v>
       </c>
-      <c r="AC55" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD55" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE55" t="n">
         <v>18.0</v>
       </c>
-      <c r="AE55" t="n">
+      <c r="AF55" t="n">
         <v>82.0</v>
+      </c>
+      <c r="AG55" t="n">
+        <v>87.0</v>
       </c>
     </row>
     <row r="56">
@@ -6412,25 +6746,31 @@
         <v>2.04</v>
       </c>
       <c r="Y56" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="Z56" t="n">
         <v>12.0</v>
       </c>
-      <c r="Z56" t="n">
+      <c r="AA56" t="n">
         <v>4.0</v>
       </c>
-      <c r="AA56" t="n">
+      <c r="AB56" t="n">
         <v>18.0</v>
       </c>
-      <c r="AB56" t="n">
+      <c r="AC56" t="n">
         <v>25.0</v>
       </c>
-      <c r="AC56" t="n">
+      <c r="AD56" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD56" t="n">
+      <c r="AE56" t="n">
         <v>18.0</v>
       </c>
-      <c r="AE56" t="n">
+      <c r="AF56" t="n">
         <v>20.0</v>
+      </c>
+      <c r="AG56" t="n">
+        <v>40.0</v>
       </c>
     </row>
     <row r="57">
@@ -6525,25 +6865,31 @@
         <v>1.7</v>
       </c>
       <c r="Y57" t="n">
+        <v>11.0</v>
+      </c>
+      <c r="Z57" t="n">
         <v>17.0</v>
       </c>
-      <c r="Z57" t="n">
+      <c r="AA57" t="n">
         <v>13.0</v>
       </c>
-      <c r="AA57" t="n">
+      <c r="AB57" t="n">
         <v>10.0</v>
       </c>
-      <c r="AB57" t="n">
+      <c r="AC57" t="n">
         <v>40.0</v>
       </c>
-      <c r="AC57" t="n">
+      <c r="AD57" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD57" t="n">
+      <c r="AE57" t="n">
         <v>25.0</v>
       </c>
-      <c r="AE57" t="n">
+      <c r="AF57" t="n">
         <v>6.0</v>
+      </c>
+      <c r="AG57" t="n">
+        <v>44.0</v>
       </c>
     </row>
     <row r="58">
@@ -6638,25 +6984,31 @@
         <v>2.68</v>
       </c>
       <c r="Y58" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="Z58" t="n">
         <v>19.0</v>
       </c>
-      <c r="Z58" t="n">
+      <c r="AA58" t="n">
         <v>12.0</v>
       </c>
-      <c r="AA58" t="n">
+      <c r="AB58" t="n">
         <v>4.0</v>
       </c>
-      <c r="AB58" t="n">
+      <c r="AC58" t="n">
         <v>43.0</v>
       </c>
-      <c r="AC58" t="n">
+      <c r="AD58" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD58" t="n">
+      <c r="AE58" t="n">
         <v>9.0</v>
       </c>
-      <c r="AE58" t="n">
+      <c r="AF58" t="n">
         <v>29.0</v>
+      </c>
+      <c r="AG58" t="n">
+        <v>49.0</v>
       </c>
     </row>
     <row r="59">
@@ -6751,25 +7103,31 @@
         <v>0.65</v>
       </c>
       <c r="Y59" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="Z59" t="n">
         <v>50.0</v>
       </c>
-      <c r="Z59" t="n">
+      <c r="AA59" t="n">
         <v>58.0</v>
       </c>
-      <c r="AA59" t="n">
+      <c r="AB59" t="n">
         <v>41.0</v>
       </c>
-      <c r="AB59" t="n">
+      <c r="AC59" t="n">
         <v>33.0</v>
       </c>
-      <c r="AC59" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD59" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE59" t="n">
         <v>25.0</v>
       </c>
-      <c r="AE59" t="n">
+      <c r="AF59" t="n">
         <v>26.0</v>
+      </c>
+      <c r="AG59" t="n">
+        <v>45.0</v>
       </c>
     </row>
     <row r="60">
@@ -6864,25 +7222,31 @@
         <v>1.89</v>
       </c>
       <c r="Y60" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="Z60" t="n">
         <v>11.0</v>
-      </c>
-      <c r="Z60" t="n">
-        <v>2.0</v>
       </c>
       <c r="AA60" t="n">
         <v>2.0</v>
       </c>
       <c r="AB60" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="AC60" t="n">
         <v>37.0</v>
       </c>
-      <c r="AC60" t="n">
+      <c r="AD60" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD60" t="n">
+      <c r="AE60" t="n">
         <v>18.0</v>
       </c>
-      <c r="AE60" t="n">
+      <c r="AF60" t="n">
         <v>71.0</v>
+      </c>
+      <c r="AG60" t="n">
+        <v>9.0</v>
       </c>
     </row>
     <row r="61">
@@ -6977,25 +7341,31 @@
         <v>1.03</v>
       </c>
       <c r="Y61" t="n">
+        <v>21.8</v>
+      </c>
+      <c r="Z61" t="n">
         <v>61.0</v>
       </c>
-      <c r="Z61" t="n">
+      <c r="AA61" t="n">
         <v>82.0</v>
       </c>
-      <c r="AA61" t="n">
+      <c r="AB61" t="n">
         <v>76.0</v>
       </c>
-      <c r="AB61" t="n">
+      <c r="AC61" t="n">
         <v>2.0</v>
       </c>
-      <c r="AC61" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD61" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE61" t="n">
         <v>72.0</v>
       </c>
-      <c r="AE61" t="n">
+      <c r="AF61" t="n">
         <v>23.0</v>
+      </c>
+      <c r="AG61" t="n">
+        <v>79.0</v>
       </c>
     </row>
     <row r="62">
@@ -7090,25 +7460,31 @@
         <v>1.51</v>
       </c>
       <c r="Y62" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="Z62" t="n">
         <v>76.0</v>
       </c>
-      <c r="Z62" t="n">
+      <c r="AA62" t="n">
         <v>74.0</v>
       </c>
-      <c r="AA62" t="n">
+      <c r="AB62" t="n">
         <v>31.0</v>
       </c>
-      <c r="AB62" t="n">
+      <c r="AC62" t="n">
         <v>80.0</v>
       </c>
-      <c r="AC62" t="n">
+      <c r="AD62" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD62" t="n">
+      <c r="AE62" t="n">
         <v>65.0</v>
       </c>
-      <c r="AE62" t="n">
+      <c r="AF62" t="n">
         <v>66.0</v>
+      </c>
+      <c r="AG62" t="n">
+        <v>72.0</v>
       </c>
     </row>
     <row r="63">
@@ -7203,25 +7579,31 @@
         <v>1.51</v>
       </c>
       <c r="Y63" t="n">
+        <v>17.9</v>
+      </c>
+      <c r="Z63" t="n">
         <v>76.0</v>
       </c>
-      <c r="Z63" t="n">
+      <c r="AA63" t="n">
         <v>74.0</v>
       </c>
-      <c r="AA63" t="n">
+      <c r="AB63" t="n">
         <v>31.0</v>
       </c>
-      <c r="AB63" t="n">
+      <c r="AC63" t="n">
         <v>80.0</v>
       </c>
-      <c r="AC63" t="n">
+      <c r="AD63" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD63" t="n">
+      <c r="AE63" t="n">
         <v>65.0</v>
       </c>
-      <c r="AE63" t="n">
+      <c r="AF63" t="n">
         <v>66.0</v>
+      </c>
+      <c r="AG63" t="n">
+        <v>72.0</v>
       </c>
     </row>
     <row r="64">
@@ -7316,25 +7698,31 @@
         <v>0.31</v>
       </c>
       <c r="Y64" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="Z64" t="n">
         <v>50.0</v>
       </c>
-      <c r="Z64" t="n">
+      <c r="AA64" t="n">
         <v>58.0</v>
       </c>
-      <c r="AA64" t="n">
+      <c r="AB64" t="n">
         <v>41.0</v>
       </c>
-      <c r="AB64" t="n">
+      <c r="AC64" t="n">
         <v>33.0</v>
       </c>
-      <c r="AC64" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD64" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE64" t="n">
         <v>57.0</v>
       </c>
-      <c r="AE64" t="n">
+      <c r="AF64" t="n">
         <v>26.0</v>
+      </c>
+      <c r="AG64" t="n">
+        <v>9.0</v>
       </c>
     </row>
     <row r="65">
@@ -7429,25 +7817,31 @@
         <v>0.75</v>
       </c>
       <c r="Y65" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="Z65" t="n">
         <v>63.0</v>
       </c>
-      <c r="Z65" t="n">
+      <c r="AA65" t="n">
         <v>56.0</v>
       </c>
-      <c r="AA65" t="n">
+      <c r="AB65" t="n">
         <v>80.0</v>
       </c>
-      <c r="AB65" t="n">
+      <c r="AC65" t="n">
         <v>67.0</v>
       </c>
-      <c r="AC65" t="n">
+      <c r="AD65" t="n">
         <v>25.0</v>
       </c>
-      <c r="AD65" t="n">
+      <c r="AE65" t="n">
         <v>57.0</v>
       </c>
-      <c r="AE65" t="n">
+      <c r="AF65" t="n">
         <v>66.0</v>
+      </c>
+      <c r="AG65" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="66">
@@ -7542,25 +7936,31 @@
         <v>1.06</v>
       </c>
       <c r="Y66" t="n">
+        <v>24.9</v>
+      </c>
+      <c r="Z66" t="n">
         <v>38.0</v>
       </c>
-      <c r="Z66" t="n">
+      <c r="AA66" t="n">
         <v>47.0</v>
       </c>
-      <c r="AA66" t="n">
+      <c r="AB66" t="n">
         <v>70.0</v>
       </c>
-      <c r="AB66" t="n">
+      <c r="AC66" t="n">
         <v>6.0</v>
       </c>
-      <c r="AC66" t="n">
+      <c r="AD66" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD66" t="n">
+      <c r="AE66" t="n">
         <v>14.0</v>
       </c>
-      <c r="AE66" t="n">
+      <c r="AF66" t="n">
         <v>30.0</v>
+      </c>
+      <c r="AG66" t="n">
+        <v>84.0</v>
       </c>
     </row>
     <row r="67">
@@ -7655,25 +8055,31 @@
         <v>2.26</v>
       </c>
       <c r="Y67" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="Z67" t="n">
         <v>15.0</v>
       </c>
-      <c r="Z67" t="n">
+      <c r="AA67" t="n">
         <v>16.0</v>
       </c>
-      <c r="AA67" t="n">
+      <c r="AB67" t="n">
         <v>27.0</v>
       </c>
-      <c r="AB67" t="n">
+      <c r="AC67" t="n">
         <v>10.0</v>
       </c>
-      <c r="AC67" t="n">
+      <c r="AD67" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD67" t="n">
+      <c r="AE67" t="n">
         <v>18.0</v>
       </c>
-      <c r="AE67" t="n">
+      <c r="AF67" t="n">
         <v>36.0</v>
+      </c>
+      <c r="AG67" t="n">
+        <v>31.0</v>
       </c>
     </row>
     <row r="68">
@@ -7768,25 +8174,31 @@
         <v>1.57</v>
       </c>
       <c r="Y68" t="n">
+        <v>7.6</v>
+      </c>
+      <c r="Z68" t="n">
         <v>32.0</v>
       </c>
-      <c r="Z68" t="n">
+      <c r="AA68" t="n">
         <v>15.0</v>
       </c>
-      <c r="AA68" t="n">
+      <c r="AB68" t="n">
         <v>61.0</v>
       </c>
-      <c r="AB68" t="n">
+      <c r="AC68" t="n">
         <v>64.0</v>
       </c>
-      <c r="AC68" t="n">
+      <c r="AD68" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD68" t="n">
+      <c r="AE68" t="n">
         <v>34.0</v>
       </c>
-      <c r="AE68" t="n">
+      <c r="AF68" t="n">
         <v>33.0</v>
+      </c>
+      <c r="AG68" t="n">
+        <v>22.0</v>
       </c>
     </row>
     <row r="69">
@@ -7881,25 +8293,31 @@
         <v>1.26</v>
       </c>
       <c r="Y69" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="Z69" t="n">
         <v>26.0</v>
       </c>
-      <c r="Z69" t="n">
+      <c r="AA69" t="n">
         <v>20.0</v>
       </c>
-      <c r="AA69" t="n">
+      <c r="AB69" t="n">
         <v>19.0</v>
       </c>
-      <c r="AB69" t="n">
+      <c r="AC69" t="n">
         <v>41.0</v>
       </c>
-      <c r="AC69" t="n">
+      <c r="AD69" t="n">
         <v>58.0</v>
       </c>
-      <c r="AD69" t="n">
+      <c r="AE69" t="n">
         <v>51.0</v>
       </c>
-      <c r="AE69" t="n">
+      <c r="AF69" t="n">
         <v>33.0</v>
+      </c>
+      <c r="AG69" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="70">
@@ -7994,25 +8412,31 @@
         <v>3.08</v>
       </c>
       <c r="Y70" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="Z70" t="n">
         <v>5.0</v>
       </c>
-      <c r="Z70" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AA70" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AB70" t="n">
         <v>7.0</v>
       </c>
-      <c r="AB70" t="n">
+      <c r="AC70" t="n">
         <v>57.0</v>
       </c>
-      <c r="AC70" t="n">
+      <c r="AD70" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD70" t="n">
+      <c r="AE70" t="n">
         <v>2.0</v>
       </c>
-      <c r="AE70" t="n">
+      <c r="AF70" t="n">
         <v>50.0</v>
+      </c>
+      <c r="AG70" t="n">
+        <v>6.0</v>
       </c>
     </row>
     <row r="71">
@@ -8107,25 +8531,31 @@
         <v>1.89</v>
       </c>
       <c r="Y71" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="Z71" t="n">
         <v>67.0</v>
       </c>
-      <c r="Z71" t="n">
+      <c r="AA71" t="n">
         <v>68.0</v>
       </c>
-      <c r="AA71" t="n">
+      <c r="AB71" t="n">
         <v>39.0</v>
       </c>
-      <c r="AB71" t="n">
+      <c r="AC71" t="n">
         <v>61.0</v>
       </c>
-      <c r="AC71" t="n">
+      <c r="AD71" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD71" t="n">
+      <c r="AE71" t="n">
         <v>11.0</v>
       </c>
-      <c r="AE71" t="n">
+      <c r="AF71" t="n">
         <v>69.0</v>
+      </c>
+      <c r="AG71" t="n">
+        <v>29.0</v>
       </c>
     </row>
     <row r="72">
@@ -8220,25 +8650,31 @@
         <v>2.09</v>
       </c>
       <c r="Y72" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="Z72" t="n">
         <v>20.0</v>
       </c>
-      <c r="Z72" t="n">
+      <c r="AA72" t="n">
         <v>7.0</v>
       </c>
-      <c r="AA72" t="n">
+      <c r="AB72" t="n">
         <v>23.0</v>
       </c>
-      <c r="AB72" t="n">
+      <c r="AC72" t="n">
         <v>44.0</v>
       </c>
-      <c r="AC72" t="n">
+      <c r="AD72" t="n">
         <v>59.0</v>
       </c>
-      <c r="AD72" t="n">
+      <c r="AE72" t="n">
         <v>57.0</v>
       </c>
-      <c r="AE72" t="n">
+      <c r="AF72" t="n">
         <v>8.0</v>
+      </c>
+      <c r="AG72" t="n">
+        <v>11.0</v>
       </c>
     </row>
     <row r="73">
@@ -8333,25 +8769,31 @@
         <v>2.02</v>
       </c>
       <c r="Y73" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="Z73" t="n">
         <v>41.0</v>
       </c>
-      <c r="Z73" t="n">
+      <c r="AA73" t="n">
         <v>43.0</v>
       </c>
-      <c r="AA73" t="n">
+      <c r="AB73" t="n">
         <v>75.0</v>
       </c>
-      <c r="AB73" t="n">
+      <c r="AC73" t="n">
         <v>22.0</v>
       </c>
-      <c r="AC73" t="n">
+      <c r="AD73" t="n">
         <v>72.0</v>
       </c>
-      <c r="AD73" t="n">
+      <c r="AE73" t="n">
         <v>57.0</v>
       </c>
-      <c r="AE73" t="n">
+      <c r="AF73" t="n">
         <v>47.0</v>
+      </c>
+      <c r="AG73" t="n">
+        <v>16.0</v>
       </c>
     </row>
     <row r="74">
@@ -8446,25 +8888,31 @@
         <v>1.56</v>
       </c>
       <c r="Y74" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="Z74" t="n">
         <v>78.0</v>
       </c>
-      <c r="Z74" t="n">
+      <c r="AA74" t="n">
         <v>54.0</v>
       </c>
-      <c r="AA74" t="n">
+      <c r="AB74" t="n">
         <v>34.0</v>
       </c>
-      <c r="AB74" t="n">
+      <c r="AC74" t="n">
         <v>49.0</v>
       </c>
-      <c r="AC74" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD74" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE74" t="n">
         <v>65.0</v>
       </c>
-      <c r="AE74" t="n">
+      <c r="AF74" t="n">
         <v>79.0</v>
+      </c>
+      <c r="AG74" t="n">
+        <v>63.0</v>
       </c>
     </row>
     <row r="75">
@@ -8559,25 +9007,31 @@
         <v>1.56</v>
       </c>
       <c r="Y75" t="n">
+        <v>16.4</v>
+      </c>
+      <c r="Z75" t="n">
         <v>78.0</v>
       </c>
-      <c r="Z75" t="n">
+      <c r="AA75" t="n">
         <v>54.0</v>
       </c>
-      <c r="AA75" t="n">
+      <c r="AB75" t="n">
         <v>34.0</v>
       </c>
-      <c r="AB75" t="n">
+      <c r="AC75" t="n">
         <v>49.0</v>
       </c>
-      <c r="AC75" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD75" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE75" t="n">
         <v>65.0</v>
       </c>
-      <c r="AE75" t="n">
+      <c r="AF75" t="n">
         <v>79.0</v>
+      </c>
+      <c r="AG75" t="n">
+        <v>63.0</v>
       </c>
     </row>
     <row r="76">
@@ -8672,25 +9126,31 @@
         <v>2.51</v>
       </c>
       <c r="Y76" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="Z76" t="n">
         <v>42.0</v>
       </c>
-      <c r="Z76" t="n">
+      <c r="AA76" t="n">
         <v>28.0</v>
       </c>
-      <c r="AA76" t="n">
+      <c r="AB76" t="n">
         <v>69.0</v>
       </c>
-      <c r="AB76" t="n">
+      <c r="AC76" t="n">
         <v>66.0</v>
       </c>
-      <c r="AC76" t="n">
+      <c r="AD76" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD76" t="n">
+      <c r="AE76" t="n">
         <v>51.0</v>
       </c>
-      <c r="AE76" t="n">
+      <c r="AF76" t="n">
         <v>70.0</v>
+      </c>
+      <c r="AG76" t="n">
+        <v>24.0</v>
       </c>
     </row>
     <row r="77">
@@ -8785,25 +9245,31 @@
         <v>3.31</v>
       </c>
       <c r="Y77" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="Z77" t="n">
         <v>3.0</v>
       </c>
-      <c r="Z77" t="n">
+      <c r="AA77" t="n">
         <v>16.0</v>
       </c>
-      <c r="AA77" t="n">
+      <c r="AB77" t="n">
         <v>9.0</v>
       </c>
-      <c r="AB77" t="n">
+      <c r="AC77" t="n">
         <v>32.0</v>
       </c>
-      <c r="AC77" t="n">
+      <c r="AD77" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD77" t="n">
+      <c r="AE77" t="n">
         <v>34.0</v>
       </c>
-      <c r="AE77" t="n">
+      <c r="AF77" t="n">
         <v>18.0</v>
+      </c>
+      <c r="AG77" t="n">
+        <v>23.0</v>
       </c>
     </row>
     <row r="78">
@@ -8898,25 +9364,31 @@
         <v>2.06</v>
       </c>
       <c r="Y78" t="n">
+        <v>15.3</v>
+      </c>
+      <c r="Z78" t="n">
         <v>25.0</v>
       </c>
-      <c r="Z78" t="n">
+      <c r="AA78" t="n">
         <v>30.0</v>
       </c>
-      <c r="AA78" t="n">
+      <c r="AB78" t="n">
         <v>51.0</v>
       </c>
-      <c r="AB78" t="n">
+      <c r="AC78" t="n">
         <v>24.0</v>
       </c>
-      <c r="AC78" t="n">
+      <c r="AD78" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD78" t="n">
+      <c r="AE78" t="n">
         <v>16.0</v>
       </c>
-      <c r="AE78" t="n">
+      <c r="AF78" t="n">
         <v>4.0</v>
+      </c>
+      <c r="AG78" t="n">
+        <v>61.0</v>
       </c>
     </row>
     <row r="79">
@@ -9011,25 +9483,31 @@
         <v>1.52</v>
       </c>
       <c r="Y79" t="n">
+        <v>24.5</v>
+      </c>
+      <c r="Z79" t="n">
         <v>80.0</v>
       </c>
-      <c r="Z79" t="n">
+      <c r="AA79" t="n">
         <v>78.0</v>
       </c>
-      <c r="AA79" t="n">
+      <c r="AB79" t="n">
         <v>55.0</v>
       </c>
-      <c r="AB79" t="n">
+      <c r="AC79" t="n">
         <v>58.0</v>
       </c>
-      <c r="AC79" t="n">
+      <c r="AD79" t="n">
         <v>37.0</v>
       </c>
-      <c r="AD79" t="n">
+      <c r="AE79" t="n">
         <v>11.0</v>
       </c>
-      <c r="AE79" t="n">
+      <c r="AF79" t="n">
         <v>74.0</v>
+      </c>
+      <c r="AG79" t="n">
+        <v>83.0</v>
       </c>
     </row>
     <row r="80">
@@ -9124,25 +9602,31 @@
         <v>1.86</v>
       </c>
       <c r="Y80" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="Z80" t="n">
         <v>13.0</v>
       </c>
-      <c r="Z80" t="n">
+      <c r="AA80" t="n">
         <v>11.0</v>
       </c>
-      <c r="AA80" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AB80" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AC80" t="n">
         <v>16.0</v>
       </c>
-      <c r="AC80" t="n">
+      <c r="AD80" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD80" t="n">
+      <c r="AE80" t="n">
         <v>25.0</v>
       </c>
-      <c r="AE80" t="n">
+      <c r="AF80" t="n">
         <v>58.0</v>
+      </c>
+      <c r="AG80" t="n">
+        <v>36.0</v>
       </c>
     </row>
     <row r="81">
@@ -9237,25 +9721,31 @@
         <v>1.37</v>
       </c>
       <c r="Y81" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="Z81" t="n">
         <v>65.0</v>
       </c>
-      <c r="Z81" t="n">
+      <c r="AA81" t="n">
         <v>71.0</v>
       </c>
-      <c r="AA81" t="n">
+      <c r="AB81" t="n">
         <v>65.0</v>
       </c>
-      <c r="AB81" t="n">
+      <c r="AC81" t="n">
         <v>83.0</v>
       </c>
-      <c r="AC81" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD81" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE81" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE81" t="n">
+      <c r="AF81" t="n">
         <v>22.0</v>
+      </c>
+      <c r="AG81" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="82">
@@ -9350,25 +9840,31 @@
         <v>0.55</v>
       </c>
       <c r="Y82" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="Z82" t="n">
         <v>6.0</v>
       </c>
-      <c r="Z82" t="n">
+      <c r="AA82" t="n">
         <v>35.0</v>
       </c>
-      <c r="AA82" t="n">
+      <c r="AB82" t="n">
         <v>13.0</v>
       </c>
-      <c r="AB82" t="n">
+      <c r="AC82" t="n">
         <v>51.0</v>
       </c>
-      <c r="AC82" t="n">
+      <c r="AD82" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD82" t="n">
+      <c r="AE82" t="n">
         <v>3.0</v>
       </c>
-      <c r="AE82" t="n">
-        <v>1.0</v>
+      <c r="AF82" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AG82" t="n">
+        <v>81.0</v>
       </c>
     </row>
     <row r="83">
@@ -9463,25 +9959,31 @@
         <v>1.31</v>
       </c>
       <c r="Y83" t="n">
+        <v>25.6</v>
+      </c>
+      <c r="Z83" t="n">
         <v>46.0</v>
       </c>
-      <c r="Z83" t="n">
+      <c r="AA83" t="n">
         <v>45.0</v>
       </c>
-      <c r="AA83" t="n">
+      <c r="AB83" t="n">
         <v>59.0</v>
       </c>
-      <c r="AB83" t="n">
+      <c r="AC83" t="n">
         <v>28.0</v>
       </c>
-      <c r="AC83" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD83" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE83" t="n">
         <v>51.0</v>
       </c>
-      <c r="AE83" t="n">
+      <c r="AF83" t="n">
         <v>78.0</v>
+      </c>
+      <c r="AG83" t="n">
+        <v>86.0</v>
       </c>
     </row>
     <row r="84">
@@ -9576,25 +10078,31 @@
         <v>0.92</v>
       </c>
       <c r="Y84" t="n">
+        <v>22.3</v>
+      </c>
+      <c r="Z84" t="n">
         <v>6.0</v>
       </c>
-      <c r="Z84" t="n">
+      <c r="AA84" t="n">
         <v>35.0</v>
       </c>
-      <c r="AA84" t="n">
+      <c r="AB84" t="n">
         <v>13.0</v>
       </c>
-      <c r="AB84" t="n">
+      <c r="AC84" t="n">
         <v>51.0</v>
       </c>
-      <c r="AC84" t="n">
+      <c r="AD84" t="n">
         <v>74.0</v>
       </c>
-      <c r="AD84" t="n">
+      <c r="AE84" t="n">
         <v>5.0</v>
       </c>
-      <c r="AE84" t="n">
-        <v>1.0</v>
+      <c r="AF84" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AG84" t="n">
+        <v>80.0</v>
       </c>
     </row>
     <row r="85">
@@ -9689,25 +10197,31 @@
         <v>1.33</v>
       </c>
       <c r="Y85" t="n">
+        <v>13.1</v>
+      </c>
+      <c r="Z85" t="n">
         <v>56.0</v>
       </c>
-      <c r="Z85" t="n">
+      <c r="AA85" t="n">
         <v>50.0</v>
       </c>
-      <c r="AA85" t="n">
+      <c r="AB85" t="n">
         <v>81.0</v>
       </c>
-      <c r="AB85" t="n">
+      <c r="AC85" t="n">
         <v>63.0</v>
       </c>
-      <c r="AC85" t="n">
+      <c r="AD85" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD85" t="n">
+      <c r="AE85" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE85" t="n">
+      <c r="AF85" t="n">
         <v>46.0</v>
+      </c>
+      <c r="AG85" t="n">
+        <v>55.0</v>
       </c>
     </row>
     <row r="86">
@@ -9802,25 +10316,31 @@
         <v>0.41</v>
       </c>
       <c r="Y86" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="Z86" t="n">
         <v>61.0</v>
       </c>
-      <c r="Z86" t="n">
+      <c r="AA86" t="n">
         <v>82.0</v>
       </c>
-      <c r="AA86" t="n">
+      <c r="AB86" t="n">
         <v>76.0</v>
       </c>
-      <c r="AB86" t="n">
+      <c r="AC86" t="n">
         <v>2.0</v>
       </c>
-      <c r="AC86" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD86" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE86" t="n">
         <v>88.0</v>
       </c>
-      <c r="AE86" t="n">
+      <c r="AF86" t="n">
         <v>23.0</v>
+      </c>
+      <c r="AG86" t="n">
+        <v>60.0</v>
       </c>
     </row>
     <row r="87">
@@ -9915,25 +10435,31 @@
         <v>2.32</v>
       </c>
       <c r="Y87" t="n">
+        <v>9.9</v>
+      </c>
+      <c r="Z87" t="n">
         <v>58.0</v>
-      </c>
-      <c r="Z87" t="n">
-        <v>63.0</v>
       </c>
       <c r="AA87" t="n">
         <v>63.0</v>
       </c>
       <c r="AB87" t="n">
+        <v>63.0</v>
+      </c>
+      <c r="AC87" t="n">
         <v>87.0</v>
       </c>
-      <c r="AC87" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD87" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE87" t="n">
         <v>57.0</v>
       </c>
-      <c r="AE87" t="n">
+      <c r="AF87" t="n">
         <v>15.0</v>
+      </c>
+      <c r="AG87" t="n">
+        <v>37.0</v>
       </c>
     </row>
     <row r="88">
@@ -10028,25 +10554,31 @@
         <v>1.84</v>
       </c>
       <c r="Y88" t="n">
+        <v>15.7</v>
+      </c>
+      <c r="Z88" t="n">
         <v>64.0</v>
       </c>
-      <c r="Z88" t="n">
+      <c r="AA88" t="n">
         <v>65.0</v>
       </c>
-      <c r="AA88" t="n">
+      <c r="AB88" t="n">
         <v>84.0</v>
       </c>
-      <c r="AB88" t="n">
+      <c r="AC88" t="n">
         <v>54.0</v>
       </c>
-      <c r="AC88" t="n">
+      <c r="AD88" t="n">
         <v>26.0</v>
       </c>
-      <c r="AD88" t="n">
+      <c r="AE88" t="n">
         <v>78.0</v>
       </c>
-      <c r="AE88" t="n">
+      <c r="AF88" t="n">
         <v>65.0</v>
+      </c>
+      <c r="AG88" t="n">
+        <v>62.0</v>
       </c>
     </row>
     <row r="89">
@@ -10141,25 +10673,31 @@
         <v>2.05</v>
       </c>
       <c r="Y89" t="n">
+        <v>11.6</v>
+      </c>
+      <c r="Z89" t="n">
         <v>74.0</v>
       </c>
-      <c r="Z89" t="n">
+      <c r="AA89" t="n">
         <v>79.0</v>
       </c>
-      <c r="AA89" t="n">
+      <c r="AB89" t="n">
         <v>67.0</v>
       </c>
-      <c r="AB89" t="n">
+      <c r="AC89" t="n">
         <v>65.0</v>
       </c>
-      <c r="AC89" t="n">
-        <v>1.0</v>
-      </c>
       <c r="AD89" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="AE89" t="n">
         <v>34.0</v>
       </c>
-      <c r="AE89" t="n">
+      <c r="AF89" t="n">
         <v>37.0</v>
+      </c>
+      <c r="AG89" t="n">
+        <v>49.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>